<commit_message>
Quick fix, merged Kalendar onto Kalendarz_vol2
</commit_message>
<xml_diff>
--- a/cmake-build-debug/wizyty.xlsx
+++ b/cmake-build-debug/wizyty.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projekt-IO\cmake-build-debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wikto\CLionProjects\kalendarz\cmake-build-debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB7BE2B-20B8-449E-97EC-EC00A14D2E82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8E1AE1-BA25-4222-A2F8-723B257A6286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FF49B81A-127A-B44C-A44B-FF0F3EF8FCF9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14976" xr2:uid="{FF49B81A-127A-B44C-A44B-FF0F3EF8FCF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="1">
   <si>
     <t>//</t>
   </si>
@@ -47,10 +47,16 @@
     <t>2222222</t>
   </si>
   <si>
-    <t>15.22</t>
-  </si>
-  <si>
-    <t>10,01,2023</t>
+    <t>19.09.2022</t>
+  </si>
+  <si>
+    <t>19.22</t>
+  </si>
+  <si>
+    <t>wiktor.k.2002@icloud.com</t>
+  </si>
+  <si>
+    <t>01</t>
   </si>
 </sst>
 </file>
@@ -86,9 +92,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -395,7 +400,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -403,15 +408,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049FB1B4-2A61-4643-8816-8B76EC36FD4B}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -427,8 +432,14 @@
       <c r="E1" t="s">
         <v>0</v>
       </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -438,15 +449,20 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
-        <v>4</v>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
I see no changes every where i see is random errors
</commit_message>
<xml_diff>
--- a/cmake-build-debug/wizyty.xlsx
+++ b/cmake-build-debug/wizyty.xlsx
@@ -57,6 +57,45 @@
   </si>
   <si>
     <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>21323123121</t>
+  </si>
+  <si>
+    <t>20.10.2023</t>
+  </si>
+  <si>
+    <t>14.11</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>XD</t>
+  </si>
+  <si>
+    <t>xd</t>
+  </si>
+  <si>
+    <t>23121243312</t>
+  </si>
+  <si>
+    <t>20.01.2023</t>
+  </si>
+  <si>
+    <t>15.11</t>
+  </si>
+  <si>
+    <t>ddd</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
@@ -462,6 +501,75 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Button changed, added prep work for patient history
</commit_message>
<xml_diff>
--- a/cmake-build-debug/wizyty.xlsx
+++ b/cmake-build-debug/wizyty.xlsx
@@ -219,6 +219,18 @@
   </si>
   <si>
     <t>08.11</t>
+  </si>
+  <si>
+    <t>DD.MM.YYYY</t>
+  </si>
+  <si>
+    <t>HH.MM</t>
+  </si>
+  <si>
+    <t>14.14</t>
+  </si>
+  <si>
+    <t>08.10</t>
   </si>
 </sst>
 </file>
@@ -730,7 +742,7 @@
         <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F7" t="s">
         <v>14</v>

</xml_diff>